<commit_message>
reorganized, deleted irrelevant files, finetuned
</commit_message>
<xml_diff>
--- a/6ppd-q/Data/HPLC_6.xlsx
+++ b/6ppd-q/Data/HPLC_6.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4795f5e3347afba5/Desktop/Dissertation/Lake_Murray/2024-25_Lake_Murray_Bioassays/6ppd-q/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{44CFB0DC-A7B4-4300-A4A7-832CD6DB97E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEFCC8BE-5C7B-48D4-9CB6-4DE44FB6DD18}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{44CFB0DC-A7B4-4300-A4A7-832CD6DB97E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EA29ECF-C041-4BC9-9655-65094B957D5D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{4F15C88E-56BB-4DB7-B2CD-E499D21DD55A}"/>
   </bookViews>
@@ -172,8 +172,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -189,10 +189,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -515,13 +511,13 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A16"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -532,16 +528,16 @@
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -552,8 +548,8 @@
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3">
-        <v>45434</v>
+      <c r="C2" s="4">
+        <v>45525</v>
       </c>
       <c r="D2" s="2">
         <v>3.8393350268211348</v>
@@ -574,8 +570,8 @@
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3">
-        <v>45434</v>
+      <c r="C3" s="4">
+        <v>45525</v>
       </c>
       <c r="D3" s="2">
         <v>6.0545924753474578</v>
@@ -592,8 +588,8 @@
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3">
-        <v>45434</v>
+      <c r="C4" s="4">
+        <v>45525</v>
       </c>
       <c r="D4" s="2">
         <v>6.4282210223849283</v>
@@ -610,8 +606,8 @@
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3">
-        <v>45434</v>
+      <c r="C5" s="4">
+        <v>45525</v>
       </c>
       <c r="D5" s="2">
         <v>6.6809415954217535</v>
@@ -628,8 +624,8 @@
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3">
-        <v>45434</v>
+      <c r="C6" s="4">
+        <v>45525</v>
       </c>
       <c r="D6" s="2">
         <v>6.4093833894174699</v>
@@ -646,8 +642,8 @@
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3">
-        <v>45437</v>
+      <c r="C7" s="4">
+        <v>45528</v>
       </c>
       <c r="D7" s="2">
         <v>6.3686326564983844</v>
@@ -668,8 +664,8 @@
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3">
-        <v>45437</v>
+      <c r="C8" s="4">
+        <v>45528</v>
       </c>
       <c r="D8" s="2">
         <v>13.241892258415939</v>
@@ -686,8 +682,8 @@
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="3">
-        <v>45437</v>
+      <c r="C9" s="4">
+        <v>45528</v>
       </c>
       <c r="D9" s="2">
         <v>13.625675074341654</v>
@@ -704,8 +700,8 @@
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="3">
-        <v>45437</v>
+      <c r="C10" s="4">
+        <v>45528</v>
       </c>
       <c r="D10" s="2">
         <v>15.4173398121416</v>
@@ -722,8 +718,8 @@
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="3">
-        <v>45437</v>
+      <c r="C11" s="4">
+        <v>45528</v>
       </c>
       <c r="D11" s="2">
         <v>14.645983922873965</v>
@@ -740,8 +736,8 @@
       <c r="B12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="3">
-        <v>45437</v>
+      <c r="C12" s="4">
+        <v>45528</v>
       </c>
       <c r="D12" s="2">
         <v>29.551554067076594</v>
@@ -762,8 +758,8 @@
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="3">
-        <v>45437</v>
+      <c r="C13" s="4">
+        <v>45528</v>
       </c>
       <c r="D13" s="2">
         <v>18.229349287732109</v>
@@ -780,8 +776,8 @@
       <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="3">
-        <v>45437</v>
+      <c r="C14" s="4">
+        <v>45528</v>
       </c>
       <c r="D14" s="2">
         <v>13.742759881209464</v>
@@ -798,8 +794,8 @@
       <c r="B15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="3">
-        <v>45437</v>
+      <c r="C15" s="4">
+        <v>45528</v>
       </c>
       <c r="D15" s="2">
         <v>14.364807046245565</v>
@@ -816,8 +812,8 @@
       <c r="B16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="3">
-        <v>45437</v>
+      <c r="C16" s="4">
+        <v>45528</v>
       </c>
       <c r="D16" s="2">
         <v>14.332937182266383</v>
@@ -834,8 +830,8 @@
       <c r="B17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="3">
-        <v>45437</v>
+      <c r="C17" s="4">
+        <v>45528</v>
       </c>
       <c r="D17" s="2">
         <v>13.635037276699762</v>
@@ -856,8 +852,8 @@
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="3">
-        <v>45437</v>
+      <c r="C18" s="4">
+        <v>45528</v>
       </c>
       <c r="D18" s="2">
         <v>18.733590020849046</v>
@@ -874,8 +870,8 @@
       <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="3">
-        <v>45437</v>
+      <c r="C19" s="4">
+        <v>45528</v>
       </c>
       <c r="D19" s="2">
         <v>13.022616429967147</v>
@@ -892,8 +888,8 @@
       <c r="B20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="3">
-        <v>45437</v>
+      <c r="C20" s="4">
+        <v>45528</v>
       </c>
       <c r="D20" s="2">
         <v>10.748362646625253</v>
@@ -910,8 +906,8 @@
       <c r="B21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="3">
-        <v>45437</v>
+      <c r="C21" s="4">
+        <v>45528</v>
       </c>
       <c r="D21" s="2">
         <v>10.926798770469112</v>
@@ -928,8 +924,8 @@
       <c r="B22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="3">
-        <v>45437</v>
+      <c r="C22" s="4">
+        <v>45528</v>
       </c>
       <c r="D22" s="2">
         <v>11.335347637684297</v>
@@ -950,8 +946,8 @@
       <c r="B23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="3">
-        <v>45437</v>
+      <c r="C23" s="4">
+        <v>45528</v>
       </c>
       <c r="D23" s="2">
         <v>9.852658131053623</v>
@@ -968,8 +964,8 @@
       <c r="B24" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="3">
-        <v>45437</v>
+      <c r="C24" s="4">
+        <v>45528</v>
       </c>
       <c r="D24" s="2">
         <v>10.95013629697652</v>
@@ -986,8 +982,8 @@
       <c r="B25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="3">
-        <v>45437</v>
+      <c r="C25" s="4">
+        <v>45528</v>
       </c>
       <c r="D25" s="2">
         <v>11.515661683328675</v>
@@ -1004,8 +1000,8 @@
       <c r="B26" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="3">
-        <v>45437</v>
+      <c r="C26" s="4">
+        <v>45528</v>
       </c>
       <c r="D26" s="2">
         <v>11.270202131867402</v>
@@ -1022,8 +1018,8 @@
       <c r="B27" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="3">
-        <v>45437</v>
+      <c r="C27" s="4">
+        <v>45528</v>
       </c>
       <c r="D27" s="2">
         <v>10.04382948285614</v>
@@ -1044,8 +1040,8 @@
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="3">
-        <v>45437</v>
+      <c r="C28" s="4">
+        <v>45528</v>
       </c>
       <c r="D28" s="2">
         <v>11.973708106672625</v>
@@ -1062,8 +1058,8 @@
       <c r="B29" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="3">
-        <v>45437</v>
+      <c r="C29" s="4">
+        <v>45528</v>
       </c>
       <c r="D29" s="2">
         <v>11.255436340080541</v>
@@ -1080,8 +1076,8 @@
       <c r="B30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="3">
-        <v>45437</v>
+      <c r="C30" s="4">
+        <v>45528</v>
       </c>
       <c r="D30" s="2">
         <v>9.2699059729525395</v>
@@ -1098,8 +1094,8 @@
       <c r="B31" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="3">
-        <v>45437</v>
+      <c r="C31" s="4">
+        <v>45528</v>
       </c>
       <c r="D31" s="2">
         <v>8.9327293464154991</v>
@@ -1116,8 +1112,8 @@
       <c r="B32" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="3">
-        <v>45437</v>
+      <c r="C32" s="4">
+        <v>45528</v>
       </c>
       <c r="D32" s="2">
         <v>10.068155181970386</v>
@@ -1138,8 +1134,8 @@
       <c r="B33" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="3">
-        <v>45437</v>
+      <c r="C33" s="4">
+        <v>45528</v>
       </c>
       <c r="D33" s="2">
         <v>12.09902522592396</v>
@@ -1156,8 +1152,8 @@
       <c r="B34" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="3">
-        <v>45437</v>
+      <c r="C34" s="4">
+        <v>45528</v>
       </c>
       <c r="D34" s="2">
         <v>12.934109756009532</v>
@@ -1174,8 +1170,8 @@
       <c r="B35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="3">
-        <v>45437</v>
+      <c r="C35" s="4">
+        <v>45528</v>
       </c>
       <c r="D35" s="2">
         <v>13.412998064625242</v>
@@ -1192,8 +1188,8 @@
       <c r="B36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="3">
-        <v>45437</v>
+      <c r="C36" s="4">
+        <v>45528</v>
       </c>
       <c r="D36" s="2">
         <v>12.774071185231682</v>
@@ -1210,8 +1206,8 @@
       <c r="B37" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="3">
-        <v>45437</v>
+      <c r="C37" s="4">
+        <v>45528</v>
       </c>
       <c r="D37" s="2">
         <v>10.283586576987114</v>
@@ -1232,8 +1228,8 @@
       <c r="B38" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="3">
-        <v>45437</v>
+      <c r="C38" s="4">
+        <v>45528</v>
       </c>
       <c r="D38" s="2">
         <v>12.638186127222099</v>
@@ -1250,8 +1246,8 @@
       <c r="B39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="3">
-        <v>45437</v>
+      <c r="C39" s="4">
+        <v>45528</v>
       </c>
       <c r="D39" s="2">
         <v>11.413101977210482</v>
@@ -1268,8 +1264,8 @@
       <c r="B40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="3">
-        <v>45437</v>
+      <c r="C40" s="4">
+        <v>45528</v>
       </c>
       <c r="D40" s="2">
         <v>11.593453269984938</v>
@@ -1286,8 +1282,8 @@
       <c r="B41" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="3">
-        <v>45437</v>
+      <c r="C41" s="4">
+        <v>45528</v>
       </c>
       <c r="D41" s="2">
         <v>12.068388361543962</v>
@@ -1304,8 +1300,8 @@
       <c r="B42" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="3">
-        <v>45437</v>
+      <c r="C42" s="4">
+        <v>45528</v>
       </c>
       <c r="D42" s="2">
         <v>5.6671294692680361</v>
@@ -1326,8 +1322,8 @@
       <c r="B43" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C43" s="3">
-        <v>45437</v>
+      <c r="C43" s="4">
+        <v>45528</v>
       </c>
       <c r="D43" s="2">
         <v>7.6101486125088202</v>
@@ -1344,8 +1340,8 @@
       <c r="B44" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="3">
-        <v>45437</v>
+      <c r="C44" s="4">
+        <v>45528</v>
       </c>
       <c r="D44" s="2">
         <v>13.968619925719034</v>
@@ -1362,8 +1358,8 @@
       <c r="B45" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="3">
-        <v>45437</v>
+      <c r="C45" s="4">
+        <v>45528</v>
       </c>
       <c r="D45" s="2">
         <v>10.085440415717201</v>
@@ -1380,8 +1376,8 @@
       <c r="B46" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C46" s="3">
-        <v>45437</v>
+      <c r="C46" s="4">
+        <v>45528</v>
       </c>
       <c r="D46" s="2">
         <v>10.418736551894494</v>

</xml_diff>